<commit_message>
Lots changes, V1 video player done thanks to Malcolm Nixon Template
Lots changes, V1 video player done thanks to Malcolm Nixon Template
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac-my.sharepoint.com/personal/mhby1g21_soton_ac_uk/Documents/COURSES/Y3/COMP3200/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="162" documentId="11_F25DC773A252ABDACC104827A91955965BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CFE1FA3-2DBF-4104-9A0F-EE9E45E3B8F4}"/>
+  <xr:revisionPtr revIDLastSave="684" documentId="11_F25DC773A252ABDACC104827A91955965BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DFE9422-E568-40D9-9ADE-CE1A8BA025EC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planned" sheetId="1" r:id="rId1"/>
-    <sheet name="Executed" sheetId="2" r:id="rId2"/>
+    <sheet name="Important dates" sheetId="4" r:id="rId1"/>
+    <sheet name="Planned" sheetId="1" r:id="rId2"/>
+    <sheet name="Executed" sheetId="2" r:id="rId3"/>
+    <sheet name="Combined" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="90">
   <si>
     <t>Project Management Gantt Chart</t>
   </si>
@@ -51,18 +53,6 @@
     <t>End Date</t>
   </si>
   <si>
-    <t>Software prototype research</t>
-  </si>
-  <si>
-    <t>Software prototype development</t>
-  </si>
-  <si>
-    <t>Revise Project Brief</t>
-  </si>
-  <si>
-    <t>Hardware prototype research</t>
-  </si>
-  <si>
     <t>Literature research</t>
   </si>
   <si>
@@ -90,15 +80,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Software prototype test</t>
-  </si>
-  <si>
-    <t>Hardware prototype documentation</t>
-  </si>
-  <si>
-    <t>Design document drafting</t>
-  </si>
-  <si>
     <t>GoDot first, then Unity, check simple way to get SBS video player and environment</t>
   </si>
   <si>
@@ -112,6 +93,222 @@
   </si>
   <si>
     <t>RancidMilkGames/Godot-VLC: An example Godot 4 project demonstrating integration with libVLCSharp (github.com)</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Revise Project Brief v1</t>
+  </si>
+  <si>
+    <t>Done v2</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>Actual Duration</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Agreed Project Brief</t>
+  </si>
+  <si>
+    <t>Deadline</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>SUBMIT a one-page PDF</t>
+  </si>
+  <si>
+    <t>Progress Report</t>
+  </si>
+  <si>
+    <t>SUBMIT a max 3000 words pdf</t>
+  </si>
+  <si>
+    <t>Final Project Report</t>
+  </si>
+  <si>
+    <t>SUBMIT final report and related files</t>
+  </si>
+  <si>
+    <t>Project Viva</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>PRESENT project demo</t>
+  </si>
+  <si>
+    <t>ELEC3227 CW</t>
+  </si>
+  <si>
+    <t>Download all related specs and datasheet to a folder.</t>
+  </si>
+  <si>
+    <t>Color Code</t>
+  </si>
+  <si>
+    <t>Orange: Report related</t>
+  </si>
+  <si>
+    <t>Green: Hardware related</t>
+  </si>
+  <si>
+    <t>Blue: Software related</t>
+  </si>
+  <si>
+    <t>Tested conversion of mp4 to .ogg with ffmpeg</t>
+  </si>
+  <si>
+    <t>Done VR screen video player like utube tutorial above but no stereo implementation yet</t>
+  </si>
+  <si>
+    <t>p1 refers to phase 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hardware procurement  </t>
+  </si>
+  <si>
+    <t>Software prototype research p1 (SPR1)</t>
+  </si>
+  <si>
+    <t>Software prototype development p1 (SPDEV1)</t>
+  </si>
+  <si>
+    <t>Software prototype test p1 (SPT1)</t>
+  </si>
+  <si>
+    <t>Hardware prototype research p1 (HPR1)</t>
+  </si>
+  <si>
+    <t>Hardware prototype documentation p1 (HPDOC1)</t>
+  </si>
+  <si>
+    <t>Design document drafting p1 (DD1)</t>
+  </si>
+  <si>
+    <t>finalise initial design and feasibility to start get hardware</t>
+  </si>
+  <si>
+    <t>read, and download all related specs and datasheet and put into a folder</t>
+  </si>
+  <si>
+    <t>submit request and wait till get component</t>
+  </si>
+  <si>
+    <t>Draft Project Report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start drafting on latex </t>
+  </si>
+  <si>
+    <t>Software prototype documentation (SPDOC1)</t>
+  </si>
+  <si>
+    <t>Write down related thing into design document and thoughts</t>
+  </si>
+  <si>
+    <t>Try leave the pico plugged in/battery powered test and see timelapse create (mono)</t>
+  </si>
+  <si>
+    <t>SPR2: Stereo and OpenXR implementation</t>
+  </si>
+  <si>
+    <t>SPDEV2: Stereo image and video</t>
+  </si>
+  <si>
+    <t>Embedded Hardware Programming study</t>
+  </si>
+  <si>
+    <t>Learn embedded programming for rasp pi pico and related interfaces for components im using</t>
+  </si>
+  <si>
+    <t>Hardware prototype testing (HPT1): Mono Testing</t>
+  </si>
+  <si>
+    <t>Hardware prototype development (HPDEV1): Basic Mono Functions</t>
+  </si>
+  <si>
+    <t>HPDOC2: Reflections and problems faced</t>
+  </si>
+  <si>
+    <t>SPDEV3: Image timelapse browsing (mono) and video playback (UI)</t>
+  </si>
+  <si>
+    <t>SPT2: Stereo 3DS video and image test</t>
+  </si>
+  <si>
+    <t>SPT3: Pico Camera images and video test (resolution changes)</t>
+  </si>
+  <si>
+    <t>HPR2: 3D Modelling Software Study and training</t>
+  </si>
+  <si>
+    <t>EXAM WEEKS</t>
+  </si>
+  <si>
+    <t>HPDEV2: 3D model design v1</t>
+  </si>
+  <si>
+    <t>HPDEV3: Stereo camera functionality</t>
+  </si>
+  <si>
+    <t>If 3d model design not yet done, can use the remaining exam weeks day</t>
+  </si>
+  <si>
+    <t>HPT3: Functional hardware test to get footage</t>
+  </si>
+  <si>
+    <t>in tandem in case problems occus midway</t>
+  </si>
+  <si>
+    <t>SPT3: Testing on friends for feedback</t>
+  </si>
+  <si>
+    <t>might still uses powerbank for power at this point, unless dev is faster</t>
+  </si>
+  <si>
+    <t>Get the basic implementation working (camera picture, video, audio and sdcard support) mono camera for now, then test with signal (control pico)</t>
+  </si>
+  <si>
+    <t>SPDEV3: Stereo audio sync and optimisation</t>
+  </si>
+  <si>
+    <t>HPDEV4: Add onboard battery (and charging circuit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HPT4: Test onboard battery life and powermode </t>
+  </si>
+  <si>
+    <t>Optimisation and organisation</t>
+  </si>
+  <si>
+    <t>Final report write up</t>
+  </si>
+  <si>
+    <t>Most likely a combination of 3 raspberry pi pico W, 1 for control and sync, 2 for hosting arducam, microphone and sdcard</t>
+  </si>
+  <si>
+    <t>PRESENT Embedded Network Coursework demo</t>
+  </si>
+  <si>
+    <t>What's the correct way to power one pi pico using another? : raspberrypipico (reddit.com)</t>
   </si>
 </sst>
 </file>
@@ -156,11 +353,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -224,30 +423,111 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Planned!$A$4:$A$7</c:f>
+              <c:f>Planned!$A$4:$A$54</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>Literature research</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Revise Project Brief</c:v>
+                  <c:v>Revise Project Brief v1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Software prototype research</c:v>
+                  <c:v>Software prototype research p1 (SPR1)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Software prototype development</c:v>
+                  <c:v>Software prototype development p1 (SPDEV1)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Software prototype test p1 (SPT1)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Hardware prototype research p1 (HPR1)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Hardware prototype documentation p1 (HPDOC1)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Design document drafting p1 (DD1)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Draft Project Report</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Hardware procurement  </c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>SPR2: Stereo and OpenXR implementation</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Software prototype documentation (SPDOC1)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>SPDEV2: Stereo image and video</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>SPT2: Stereo 3DS video and image test</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Embedded Hardware Programming study</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Hardware prototype development (HPDEV1): Basic Mono Functions</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Hardware prototype testing (HPT1): Mono Testing</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>HPDOC2: Reflections and problems faced</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>SPDEV3: Image timelapse browsing (mono) and video playback (UI)</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>SPT3: Pico Camera images and video test (resolution changes)</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>HPR2: 3D Modelling Software Study and training</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>HPDEV2: 3D model design v1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>EXAM WEEKS</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>HPDEV3: Stereo camera functionality</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>HPT3: Functional hardware test to get footage</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>SPDEV3: Stereo audio sync and optimisation</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>SPT3: Testing on friends for feedback</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>HPDEV4: Add onboard battery (and charging circuit)</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>HPT4: Test onboard battery life and powermode </c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Optimisation and organisation</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Final report write up</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planned!$B$4:$B$7</c:f>
+              <c:f>Planned!$B$4:$B$34</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>45201</c:v>
                 </c:pt>
@@ -259,6 +539,87 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>45203</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45205</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45207</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45209</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45211</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45212</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45215</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45216</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45223</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45218</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45232</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45235</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45242</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>45256</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>45259</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>45261</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>45275</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="d\-mmm">
+                  <c:v>45280</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>45294</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>45299</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>45320</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>45327</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>45334</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>45341</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>45344</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>45354</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>45361</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>45366</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -293,32 +654,569 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-1B7F-4994-A620-2F67083514CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-1B7F-4994-A620-2F67083514CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-1B7F-4994-A620-2F67083514CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-1B7F-4994-A620-2F67083514CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-1B7F-4994-A620-2F67083514CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-1B7F-4994-A620-2F67083514CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-1B7F-4994-A620-2F67083514CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-1B7F-4994-A620-2F67083514CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-1B7F-4994-A620-2F67083514CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-1B7F-4994-A620-2F67083514CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-1B7F-4994-A620-2F67083514CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-1B7F-4994-A620-2F67083514CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="16"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000C-1B7F-4994-A620-2F67083514CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="18"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-1B7F-4994-A620-2F67083514CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="19"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000E-1B7F-4994-A620-2F67083514CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="20"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-1B7F-4994-A620-2F67083514CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="21"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000010-1B7F-4994-A620-2F67083514CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="22"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-1B7F-4994-A620-2F67083514CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="23"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000012-1B7F-4994-A620-2F67083514CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="24"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-1B7F-4994-A620-2F67083514CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="25"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000014-1B7F-4994-A620-2F67083514CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="26"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-1B7F-4994-A620-2F67083514CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="27"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000016-1B7F-4994-A620-2F67083514CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="28"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-1B7F-4994-A620-2F67083514CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Planned!$A$4:$A$7</c:f>
+              <c:f>Planned!$A$4:$A$54</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>Literature research</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Revise Project Brief</c:v>
+                  <c:v>Revise Project Brief v1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Software prototype research</c:v>
+                  <c:v>Software prototype research p1 (SPR1)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Software prototype development</c:v>
+                  <c:v>Software prototype development p1 (SPDEV1)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Software prototype test p1 (SPT1)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Hardware prototype research p1 (HPR1)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Hardware prototype documentation p1 (HPDOC1)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Design document drafting p1 (DD1)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Draft Project Report</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Hardware procurement  </c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>SPR2: Stereo and OpenXR implementation</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Software prototype documentation (SPDOC1)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>SPDEV2: Stereo image and video</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>SPT2: Stereo 3DS video and image test</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Embedded Hardware Programming study</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Hardware prototype development (HPDEV1): Basic Mono Functions</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Hardware prototype testing (HPT1): Mono Testing</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>HPDOC2: Reflections and problems faced</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>SPDEV3: Image timelapse browsing (mono) and video playback (UI)</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>SPT3: Pico Camera images and video test (resolution changes)</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>HPR2: 3D Modelling Software Study and training</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>HPDEV2: 3D model design v1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>EXAM WEEKS</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>HPDEV3: Stereo camera functionality</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>HPT3: Functional hardware test to get footage</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>SPDEV3: Stereo audio sync and optimisation</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>SPT3: Testing on friends for feedback</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>HPDEV4: Add onboard battery (and charging circuit)</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>HPT4: Test onboard battery life and powermode </c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Optimisation and organisation</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Final report write up</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planned!$C$4:$C$7</c:f>
+              <c:f>Planned!$C$4:$C$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -330,6 +1228,87 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -348,7 +1327,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="52"/>
         <c:overlap val="100"/>
         <c:axId val="204364287"/>
         <c:axId val="1678321263"/>
@@ -408,6 +1387,7 @@
         <c:axId val="1678321263"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="45200"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
@@ -425,6 +1405,20 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:numFmt formatCode="d\-mmm\-yy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -557,30 +1551,42 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Planned!$A$4:$A$7</c:f>
+              <c:f>Planned!$A$4:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Literature research</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Revise Project Brief</c:v>
+                  <c:v>Revise Project Brief v1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Software prototype research</c:v>
+                  <c:v>Software prototype research p1 (SPR1)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Software prototype development</c:v>
+                  <c:v>Software prototype development p1 (SPDEV1)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Software prototype test p1 (SPT1)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Hardware prototype research p1 (HPR1)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Hardware prototype documentation p1 (HPDOC1)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Design document drafting p1 (DD1)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planned!$B$4:$B$7</c:f>
+              <c:f>Planned!$B$4:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>45201</c:v>
                 </c:pt>
@@ -592,6 +1598,18 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>45203</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45205</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45207</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45209</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -626,43 +1644,162 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-5AA4-417F-9173-E865485997FC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-5AA4-417F-9173-E865485997FC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-5AA4-417F-9173-E865485997FC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-5AA4-417F-9173-E865485997FC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-5AA4-417F-9173-E865485997FC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Planned!$A$4:$A$7</c:f>
+              <c:f>Planned!$A$4:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Literature research</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Revise Project Brief</c:v>
+                  <c:v>Revise Project Brief v1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Software prototype research</c:v>
+                  <c:v>Software prototype research p1 (SPR1)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Software prototype development</c:v>
+                  <c:v>Software prototype development p1 (SPDEV1)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Software prototype test p1 (SPT1)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Hardware prototype research p1 (HPR1)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Hardware prototype documentation p1 (HPDOC1)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Design document drafting p1 (DD1)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Executed!$C$4:$C$7</c:f>
+              <c:f>Executed!$C$4:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -670,6 +1807,666 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-28AE-4BAF-9C9E-15CCC4960187}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="204364287"/>
+        <c:axId val="1678321263"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="204364287"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1678321263"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1678321263"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="45200"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="d\-mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="204364287"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planned!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Start Date</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Executed!$A$4:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Literature research</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Revise Project Brief v1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Software prototype research p1 (SPR1)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Software prototype development p1 (SPDEV1)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Software prototype test p1 (SPT1)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Hardware prototype research p1 (HPR1)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Hardware prototype documentation p1 (HPDOC1)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Design document drafting p1 (DD1)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planned!$B$4:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>45201</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45201</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45201</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45203</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45205</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45207</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45209</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45211</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F621-4088-8188-D51CF8D00765}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Combined!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Expected Duration (days)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-F621-4088-8188-D51CF8D00765}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-F621-4088-8188-D51CF8D00765}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-F621-4088-8188-D51CF8D00765}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-F621-4088-8188-D51CF8D00765}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-F621-4088-8188-D51CF8D00765}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Executed!$A$4:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Literature research</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Revise Project Brief v1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Software prototype research p1 (SPR1)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Software prototype development p1 (SPDEV1)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Software prototype test p1 (SPT1)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Hardware prototype research p1 (HPR1)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Hardware prototype documentation p1 (HPDOC1)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Design document drafting p1 (DD1)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Combined!$C$4:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F621-4088-8188-D51CF8D00765}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Combined!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Difference</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-F621-4088-8188-D51CF8D00765}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-F621-4088-8188-D51CF8D00765}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-F621-4088-8188-D51CF8D00765}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-F621-4088-8188-D51CF8D00765}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Executed!$A$4:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Literature research</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Revise Project Brief v1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Software prototype research p1 (SPR1)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Software prototype development p1 (SPDEV1)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Software prototype test p1 (SPT1)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Hardware prototype research p1 (HPR1)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Hardware prototype documentation p1 (HPDOC1)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Design document drafting p1 (DD1)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Combined!$E$4:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F621-4088-8188-D51CF8D00765}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -925,6 +2722,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -1935,20 +3772,525 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>380999</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>157161</xdr:rowOff>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1980,16 +4322,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>147636</xdr:rowOff>
+      <xdr:rowOff>71436</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1997,6 +4339,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5C0BE40-F7F2-4B6E-ADF3-D28CF9196D4D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>97877</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>84739</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>316953</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>32350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16119625-6ACC-4193-A386-D5CEE68B5A85}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2281,8 +4666,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE445F25-8786-474F-A734-10FE3FF0DEE5}">
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
@@ -2290,18 +4675,262 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45212</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45271</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45272</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45412</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45428</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I43"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="67.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2309,24 +4938,24 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>45201</v>
@@ -2340,19 +4969,19 @@
       </c>
       <c r="E4" s="2">
         <f>Executed!E4</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="F4" t="str">
         <f>Executed!F4</f>
         <v>No</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1">
         <v>45201</v>
@@ -2361,24 +4990,27 @@
         <v>3</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" ref="D5:D11" si="0">B5+C5</f>
+        <f t="shared" ref="D5:D43" si="0">B5+C5</f>
         <v>45204</v>
       </c>
       <c r="E5" s="2">
         <f>Executed!E5</f>
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="str">
         <f>Executed!F5</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="B6" s="1">
         <v>45201</v>
@@ -2392,22 +5024,22 @@
       </c>
       <c r="E6" s="2">
         <f>Executed!E6</f>
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F6" t="str">
         <f>Executed!F6</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="B7" s="1">
         <v>45203</v>
@@ -2421,16 +5053,16 @@
       </c>
       <c r="E7" s="2">
         <f>Executed!E7</f>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F7" t="str">
         <f>Executed!F7</f>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="B8" s="1">
         <v>45205</v>
@@ -2444,16 +5076,16 @@
       </c>
       <c r="E8" s="2">
         <f>Executed!E8</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" t="str">
         <f>Executed!F8</f>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="B9" s="1">
         <v>45207</v>
@@ -2467,16 +5099,19 @@
       </c>
       <c r="E9" s="2">
         <f>Executed!E9</f>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="F9" t="str">
         <f>Executed!F9</f>
         <v>No</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="B10" s="1">
         <v>45209</v>
@@ -2496,20 +5131,23 @@
         <f>Executed!F10</f>
         <v>No</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1">
-        <v>45212</v>
+        <v>45211</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>45217</v>
+        <v>45214</v>
       </c>
       <c r="E11" s="2">
         <f>Executed!E11</f>
@@ -2518,6 +5156,432 @@
       <c r="F11" t="str">
         <f>Executed!F11</f>
         <v>No</v>
+      </c>
+      <c r="G11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="1">
+        <v>45212</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>45214</v>
+      </c>
+      <c r="G12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="1">
+        <v>45215</v>
+      </c>
+      <c r="C13">
+        <v>14</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>45229</v>
+      </c>
+      <c r="G13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="1">
+        <v>45216</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>45223</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="1">
+        <v>45223</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>45230</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="1">
+        <v>45218</v>
+      </c>
+      <c r="C16">
+        <v>14</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>45232</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="1">
+        <v>45232</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>45235</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="1">
+        <v>45235</v>
+      </c>
+      <c r="C18">
+        <v>7</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>45242</v>
+      </c>
+      <c r="G18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="1">
+        <v>45242</v>
+      </c>
+      <c r="C19">
+        <v>14</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>45256</v>
+      </c>
+      <c r="G19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="1">
+        <v>45256</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>45259</v>
+      </c>
+      <c r="G20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="1">
+        <v>45259</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>45261</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="1">
+        <v>45261</v>
+      </c>
+      <c r="C22">
+        <v>14</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>45275</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="1">
+        <v>45275</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="0"/>
+        <v>45278</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="5">
+        <v>45280</v>
+      </c>
+      <c r="C24">
+        <v>14</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="0"/>
+        <v>45294</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="1">
+        <v>45294</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="0"/>
+        <v>45299</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="1">
+        <v>45299</v>
+      </c>
+      <c r="C26">
+        <v>21</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="0"/>
+        <v>45320</v>
+      </c>
+      <c r="G26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="1">
+        <v>45320</v>
+      </c>
+      <c r="C27">
+        <v>14</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="0"/>
+        <v>45334</v>
+      </c>
+      <c r="G27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="1">
+        <v>45327</v>
+      </c>
+      <c r="C28">
+        <v>7</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="0"/>
+        <v>45334</v>
+      </c>
+      <c r="G28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="1">
+        <v>45334</v>
+      </c>
+      <c r="C29">
+        <v>7</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="0"/>
+        <v>45341</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="1">
+        <v>45341</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="0"/>
+        <v>45344</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="1">
+        <v>45344</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="0"/>
+        <v>45354</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" s="1">
+        <v>45354</v>
+      </c>
+      <c r="C32">
+        <v>7</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="0"/>
+        <v>45361</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" s="1">
+        <v>45361</v>
+      </c>
+      <c r="C33">
+        <v>5</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="0"/>
+        <v>45366</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" s="1">
+        <v>45366</v>
+      </c>
+      <c r="C34">
+        <v>21</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="0"/>
+        <v>45387</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2529,17 +5593,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F12609-C238-4402-9A8B-B1D994A238B7}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.28515625" customWidth="1"/>
+    <col min="1" max="1" width="61.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -2549,6 +5613,21 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2558,19 +5637,19 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2583,188 +5662,677 @@
         <v>45201</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1">
         <f>B4+C4</f>
-        <v>45204</v>
+        <v>45208</v>
       </c>
       <c r="E4" s="2">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>Planned!A5</f>
-        <v>Revise Project Brief</v>
+        <v>Revise Project Brief v1</v>
       </c>
       <c r="B5" s="1">
         <f>Planned!B5</f>
         <v>45201</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" ref="D5:D11" si="0">B5+C5</f>
-        <v>45204</v>
+        <v>45207</v>
       </c>
       <c r="E5" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>Planned!A6</f>
-        <v>Software prototype research</v>
+        <v>Software prototype research p1 (SPR1)</v>
       </c>
       <c r="B6" s="1">
         <f>Planned!B6</f>
         <v>45201</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>45204</v>
+        <v>45208</v>
       </c>
       <c r="E6" s="2">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>Planned!A7</f>
-        <v>Software prototype development</v>
+        <v>Software prototype development p1 (SPDEV1)</v>
       </c>
       <c r="B7" s="1">
         <f>Planned!B7</f>
         <v>45203</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>45204</v>
+        <v>45208</v>
       </c>
       <c r="E7" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>Planned!A8</f>
-        <v>Software prototype test</v>
+        <v>Software prototype test p1 (SPT1)</v>
       </c>
       <c r="B8" s="1">
         <f>Planned!B8</f>
         <v>45205</v>
       </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>45205</v>
+        <v>45208</v>
       </c>
       <c r="E8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>Planned!A9</f>
-        <v>Hardware prototype research</v>
+        <v>Hardware prototype research p1 (HPR1)</v>
       </c>
       <c r="B9" s="1">
         <f>Planned!B9</f>
         <v>45207</v>
       </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>45207</v>
+        <v>45208</v>
       </c>
       <c r="E9" s="2">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>Planned!A10</f>
-        <v>Hardware prototype documentation</v>
+        <v>Hardware prototype documentation p1 (HPDOC1)</v>
       </c>
       <c r="B10" s="1">
-        <f>Planned!B10</f>
-        <v>45209</v>
+        <v>45210</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>45209</v>
+        <v>45211</v>
       </c>
       <c r="E10" s="2">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>Planned!A11</f>
-        <v>Design document drafting</v>
+        <v>Design document drafting p1 (DD1)</v>
       </c>
       <c r="B11" s="1">
         <f>Planned!B11</f>
-        <v>45212</v>
+        <v>45211</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>45212</v>
+        <v>45211</v>
       </c>
       <c r="E11" s="2">
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>16</v>
+        <v>12</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" t="str">
         <f>Planned!A12</f>
-        <v>0</v>
+        <v>Draft Project Report</v>
+      </c>
+      <c r="B12" s="1">
+        <f>Planned!B12</f>
+        <v>45212</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f>Planned!A13</f>
+        <v xml:space="preserve">Hardware procurement  </v>
+      </c>
+      <c r="B13" s="1">
+        <f>Planned!B13</f>
+        <v>45215</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f>Planned!A14</f>
+        <v>SPR2: Stereo and OpenXR implementation</v>
+      </c>
+      <c r="B14" s="1">
+        <f>Planned!B14</f>
+        <v>45216</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f>Planned!A15</f>
+        <v>Software prototype documentation (SPDOC1)</v>
+      </c>
+      <c r="B15" s="1">
+        <f>Planned!B15</f>
+        <v>45223</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f>Planned!A16</f>
+        <v>SPDEV2: Stereo image and video</v>
+      </c>
+      <c r="B16" s="1">
+        <f>Planned!B16</f>
+        <v>45218</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f>Planned!A17</f>
+        <v>SPT2: Stereo 3DS video and image test</v>
+      </c>
+      <c r="B17" s="1">
+        <f>Planned!B17</f>
+        <v>45232</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f>Planned!A18</f>
+        <v>Embedded Hardware Programming study</v>
+      </c>
+      <c r="B18" s="1">
+        <f>Planned!B18</f>
+        <v>45235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f>Planned!A19</f>
+        <v>Hardware prototype development (HPDEV1): Basic Mono Functions</v>
+      </c>
+      <c r="B19" s="1">
+        <f>Planned!B19</f>
+        <v>45242</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f>Planned!A20</f>
+        <v>Hardware prototype testing (HPT1): Mono Testing</v>
+      </c>
+      <c r="B20" s="1">
+        <f>Planned!B20</f>
+        <v>45256</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f>Planned!A21</f>
+        <v>HPDOC2: Reflections and problems faced</v>
+      </c>
+      <c r="B21" s="1">
+        <f>Planned!B21</f>
+        <v>45259</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f>Planned!A22</f>
+        <v>SPDEV3: Image timelapse browsing (mono) and video playback (UI)</v>
+      </c>
+      <c r="B22" s="1">
+        <f>Planned!B22</f>
+        <v>45261</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f>Planned!A23</f>
+        <v>SPT3: Pico Camera images and video test (resolution changes)</v>
+      </c>
+      <c r="B23" s="1">
+        <f>Planned!B23</f>
+        <v>45275</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f>Planned!A24</f>
+        <v>HPR2: 3D Modelling Software Study and training</v>
+      </c>
+      <c r="B24" s="1">
+        <f>Planned!B24</f>
+        <v>45280</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f>Planned!A25</f>
+        <v>HPDEV2: 3D model design v1</v>
+      </c>
+      <c r="B25" s="1">
+        <f>Planned!B25</f>
+        <v>45294</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f>Planned!A26</f>
+        <v>EXAM WEEKS</v>
+      </c>
+      <c r="B26" s="1">
+        <f>Planned!B26</f>
+        <v>45299</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f>Planned!A27</f>
+        <v>HPDEV3: Stereo camera functionality</v>
+      </c>
+      <c r="B27" s="1">
+        <f>Planned!B27</f>
+        <v>45320</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f>Planned!A28</f>
+        <v>HPT3: Functional hardware test to get footage</v>
+      </c>
+      <c r="B28" s="1">
+        <f>Planned!B28</f>
+        <v>45327</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
+        <f>Planned!A29</f>
+        <v>SPDEV3: Stereo audio sync and optimisation</v>
+      </c>
+      <c r="B29" s="1">
+        <f>Planned!B29</f>
+        <v>45334</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <f>Planned!A30</f>
+        <v>SPT3: Testing on friends for feedback</v>
+      </c>
+      <c r="B30" s="1">
+        <f>Planned!B30</f>
+        <v>45341</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="str">
+        <f>Planned!A31</f>
+        <v>HPDEV4: Add onboard battery (and charging circuit)</v>
+      </c>
+      <c r="B31" s="1">
+        <f>Planned!B31</f>
+        <v>45344</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="str">
+        <f>Planned!A32</f>
+        <v xml:space="preserve">HPT4: Test onboard battery life and powermode </v>
+      </c>
+      <c r="B32" s="1">
+        <f>Planned!B32</f>
+        <v>45354</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="str">
+        <f>Planned!A33</f>
+        <v>Optimisation and organisation</v>
+      </c>
+      <c r="B33" s="1">
+        <f>Planned!B33</f>
+        <v>45361</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="str">
+        <f>Planned!A34</f>
+        <v>Final report write up</v>
+      </c>
+      <c r="B34" s="1">
+        <f>Planned!B34</f>
+        <v>45366</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I6" r:id="rId1" display="https://www.reddit.com/r/godot/comments/16zmd7s/do_godot_4_have_inbuilt_vr_video_sbs3d_player/" xr:uid="{843A9FD5-96FD-4C17-B96F-9417B6058DFD}"/>
+    <hyperlink ref="H6" r:id="rId2" xr:uid="{BF56C42D-36A8-4251-B5EB-67FB4C43AD5B}"/>
+    <hyperlink ref="G11" r:id="rId3" display="https://www.reddit.com/r/raspberrypipico/comments/pkcckg/whats_the_correct_way_to_power_one_pi_pico_using/" xr:uid="{2D460838-79B2-44ED-AE52-FCF3725BFA3F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FB32B44-AF31-4750-897C-7301F24D334D}">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1"/>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f>Executed!A4</f>
+        <v>Literature research</v>
+      </c>
+      <c r="B4" s="1">
+        <f>Executed!B4</f>
+        <v>45201</v>
+      </c>
+      <c r="C4">
+        <f>Planned!C4</f>
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <f>Executed!C4</f>
+        <v>7</v>
+      </c>
+      <c r="E4" s="4">
+        <f>IF(D4-C4&lt;0, 0, D4-C4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f>Executed!A5</f>
+        <v>Revise Project Brief v1</v>
+      </c>
+      <c r="B5" s="1">
+        <f>Executed!B5</f>
+        <v>45201</v>
+      </c>
+      <c r="C5">
+        <f>Planned!C5</f>
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <f>Executed!C5</f>
+        <v>6</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" ref="E5:E11" si="0">IF(D5-C5&lt;0, 0, D5-C5)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f>Executed!A6</f>
+        <v>Software prototype research p1 (SPR1)</v>
+      </c>
+      <c r="B6" s="1">
+        <f>Executed!B6</f>
+        <v>45201</v>
+      </c>
+      <c r="C6">
+        <f>Planned!C6</f>
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <f>Executed!C6</f>
+        <v>7</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f>Executed!A7</f>
+        <v>Software prototype development p1 (SPDEV1)</v>
+      </c>
+      <c r="B7" s="1">
+        <f>Executed!B7</f>
+        <v>45203</v>
+      </c>
+      <c r="C7">
+        <f>Planned!C7</f>
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <f>Executed!C7</f>
+        <v>5</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f>Executed!A8</f>
+        <v>Software prototype test p1 (SPT1)</v>
+      </c>
+      <c r="B8" s="1">
+        <f>Executed!B8</f>
+        <v>45205</v>
+      </c>
+      <c r="C8">
+        <f>Planned!C8</f>
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <f>Executed!C8</f>
+        <v>3</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f>Executed!A9</f>
+        <v>Hardware prototype research p1 (HPR1)</v>
+      </c>
+      <c r="B9" s="1">
+        <f>Executed!B9</f>
+        <v>45207</v>
+      </c>
+      <c r="C9">
+        <f>Planned!C9</f>
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <f>Executed!C9</f>
+        <v>1</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f>Executed!A10</f>
+        <v>Hardware prototype documentation p1 (HPDOC1)</v>
+      </c>
+      <c r="B10" s="1">
+        <f>Executed!B10</f>
+        <v>45210</v>
+      </c>
+      <c r="C10">
+        <f>Planned!C10</f>
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <f>Executed!C10</f>
+        <v>1</v>
+      </c>
+      <c r="E10" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f>Executed!A11</f>
+        <v>Design document drafting p1 (DD1)</v>
+      </c>
+      <c r="B11" s="1">
+        <f>Executed!B11</f>
+        <v>45211</v>
+      </c>
+      <c r="C11">
+        <f>Planned!C11</f>
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <f>Executed!C11</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>